<commit_message>
update prints to follow what is going on
</commit_message>
<xml_diff>
--- a/data/input/tech_mapping_in.xlsx
+++ b/data/input/tech_mapping_in.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uab-my.sharepoint.com/personal/1361185_uab_cat/Documents/Documentos/GitHub/calliope_enbios_int/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_2611E3FEB37BCA2B912D4C8A4DAD338F7978E3AF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{553A6361-636D-4B0C-85EF-A2134402237E}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_2611E3FEB37BCA2B912D4C8A4DAD338F7978E3AF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F34BD65-976B-41EB-99B6-54CDA1E646C9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="o&amp;m" sheetId="1" r:id="rId1"/>
@@ -915,12 +915,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -950,7 +956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1012,6 +1018,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1318,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2558,50 +2565,50 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
         <v>30</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="K26" s="21">
+        <v>1</v>
+      </c>
+      <c r="L26" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M26" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="N26">
-        <v>100</v>
-      </c>
-      <c r="O26" t="s">
+      <c r="N26" s="21">
+        <v>100</v>
+      </c>
+      <c r="O26" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="21">
         <v>360000000</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="Q26" s="21" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3346,8 +3353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27541EB-72A6-42F8-B6FE-A372F470059D}">
   <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B60"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add empty inventory for pv operation
</commit_message>
<xml_diff>
--- a/data/input/tech_mapping_in.xlsx
+++ b/data/input/tech_mapping_in.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uab-my.sharepoint.com/personal/1361185_uab_cat/Documents/Documentos/GitHub/calliope_enbios_int/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="11_2611E3FEB37BCA2B912D4C8A4DAD338F7978E3AF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E318788-42D7-4FE0-9D18-1840AFA98F48}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="11_2611E3FEB37BCA2B912D4C8A4DAD338F7978E3AF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E12E7FA-A964-461C-842E-9DD79CA7DA4C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="o&amp;m" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="276">
   <si>
     <t>id</t>
   </si>
@@ -905,6 +905,15 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>solar_pv</t>
+  </si>
+  <si>
+    <t>electricity production, pv, operation (empty)</t>
+  </si>
+  <si>
+    <t>Created from scratch</t>
   </si>
 </sst>
 </file>
@@ -1380,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3524,6 +3533,56 @@
         <v>158</v>
       </c>
     </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>273</v>
+      </c>
+      <c r="C42" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" t="s">
+        <v>272</v>
+      </c>
+      <c r="H42" t="s">
+        <v>274</v>
+      </c>
+      <c r="I42" t="s">
+        <v>64</v>
+      </c>
+      <c r="J42" t="s">
+        <v>124</v>
+      </c>
+      <c r="K42" t="s">
+        <v>129</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42" t="s">
+        <v>133</v>
+      </c>
+      <c r="N42" t="s">
+        <v>138</v>
+      </c>
+      <c r="O42">
+        <v>100</v>
+      </c>
+      <c r="P42" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q42">
+        <v>100000000</v>
+      </c>
+      <c r="R42" t="s">
+        <v>275</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R41">
     <sortCondition ref="A1:A41"/>
@@ -3537,8 +3596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27541EB-72A6-42F8-B6FE-A372F470059D}">
   <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P50" sqref="P50"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4360,7 +4419,7 @@
         <v>142</v>
       </c>
       <c r="P14" s="8">
-        <f>100000/K14</f>
+        <f t="shared" ref="P14:P39" si="1">100000/K14</f>
         <v>304.8780487804878</v>
       </c>
       <c r="Q14" s="9" t="s">
@@ -4417,7 +4476,7 @@
         <v>142</v>
       </c>
       <c r="P15" s="8">
-        <f>100000/K15</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
       <c r="Q15" s="9" t="s">
@@ -4474,7 +4533,7 @@
         <v>142</v>
       </c>
       <c r="P16" s="8">
-        <f>100000/K16</f>
+        <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="Q16" s="9" t="s">
@@ -4531,7 +4590,7 @@
         <v>142</v>
       </c>
       <c r="P17" s="8">
-        <f>100000/K17</f>
+        <f t="shared" si="1"/>
         <v>100000000</v>
       </c>
       <c r="Q17" s="9" t="s">
@@ -4588,7 +4647,7 @@
         <v>142</v>
       </c>
       <c r="P18" s="8">
-        <f>100000/K18</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
       <c r="Q18" s="9" t="s">
@@ -4645,7 +4704,7 @@
         <v>142</v>
       </c>
       <c r="P19" s="8">
-        <f>100000/K19</f>
+        <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="Q19" s="9" t="s">
@@ -4702,7 +4761,7 @@
         <v>142</v>
       </c>
       <c r="P20" s="8">
-        <f>100000/K20</f>
+        <f t="shared" si="1"/>
         <v>10.95290251916758</v>
       </c>
       <c r="Q20" s="9" t="s">
@@ -4759,7 +4818,7 @@
         <v>142</v>
       </c>
       <c r="P21" s="8">
-        <f>100000/K21</f>
+        <f t="shared" si="1"/>
         <v>7.2532095452237613</v>
       </c>
       <c r="Q21" s="9" t="s">
@@ -4816,7 +4875,7 @@
         <v>142</v>
       </c>
       <c r="P22" s="8">
-        <f>100000/K22</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="Q22" s="9" t="s">
@@ -4873,7 +4932,7 @@
         <v>142</v>
       </c>
       <c r="P23" s="8">
-        <f>100000/K23</f>
+        <f t="shared" si="1"/>
         <v>175438.59649122809</v>
       </c>
       <c r="Q23" s="9" t="s">
@@ -4930,7 +4989,7 @@
         <v>142</v>
       </c>
       <c r="P24" s="8">
-        <f>100000/K24</f>
+        <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="Q24" s="9" t="s">
@@ -4987,7 +5046,7 @@
         <v>142</v>
       </c>
       <c r="P25" s="8">
-        <f>100000/K25</f>
+        <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="Q25" s="9" t="s">
@@ -5044,7 +5103,7 @@
         <v>142</v>
       </c>
       <c r="P26" s="8">
-        <f>100000/K26</f>
+        <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="Q26" s="9" t="s">
@@ -5101,7 +5160,7 @@
         <v>142</v>
       </c>
       <c r="P27" s="8">
-        <f>100000/K27</f>
+        <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="Q27" s="9" t="s">
@@ -5158,7 +5217,7 @@
         <v>142</v>
       </c>
       <c r="P28" s="8">
-        <f>100000/K28</f>
+        <f t="shared" si="1"/>
         <v>10000000</v>
       </c>
       <c r="Q28" s="9" t="s">
@@ -5215,7 +5274,7 @@
         <v>142</v>
       </c>
       <c r="P29" s="8">
-        <f>100000/K29</f>
+        <f t="shared" si="1"/>
         <v>4000000</v>
       </c>
       <c r="Q29" s="9" t="s">
@@ -5272,7 +5331,7 @@
         <v>142</v>
       </c>
       <c r="P30" s="8">
-        <f>100000/K30</f>
+        <f t="shared" si="1"/>
         <v>40000000</v>
       </c>
       <c r="Q30" s="9" t="s">
@@ -5329,7 +5388,7 @@
         <v>142</v>
       </c>
       <c r="P31" s="8">
-        <f>100000/K31</f>
+        <f t="shared" si="1"/>
         <v>10000000</v>
       </c>
       <c r="Q31" s="9" t="s">
@@ -5386,7 +5445,7 @@
         <v>142</v>
       </c>
       <c r="P32" s="8">
-        <f>100000/K32</f>
+        <f t="shared" si="1"/>
         <v>10000000</v>
       </c>
       <c r="Q32" s="9" t="s">
@@ -5443,7 +5502,7 @@
         <v>142</v>
       </c>
       <c r="P33" s="8">
-        <f>100000/K33</f>
+        <f t="shared" si="1"/>
         <v>2325581.3953488376</v>
       </c>
       <c r="Q33" s="9" t="s">
@@ -5500,7 +5559,7 @@
         <v>142</v>
       </c>
       <c r="P34" s="8">
-        <f>100000/K34</f>
+        <f t="shared" si="1"/>
         <v>40000000</v>
       </c>
       <c r="Q34" s="9" t="s">
@@ -5557,7 +5616,7 @@
         <v>142</v>
       </c>
       <c r="P35" s="8">
-        <f>100000/K35</f>
+        <f t="shared" si="1"/>
         <v>40000000</v>
       </c>
       <c r="Q35" s="9" t="s">
@@ -5614,7 +5673,7 @@
         <v>142</v>
       </c>
       <c r="P36" s="8">
-        <f>100000/K36</f>
+        <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="Q36" s="9" t="s">
@@ -5677,7 +5736,7 @@
         <v>142</v>
       </c>
       <c r="P37" s="8">
-        <f>100000/K37</f>
+        <f t="shared" si="1"/>
         <v>100000000</v>
       </c>
       <c r="Q37" s="9" t="s">
@@ -5734,7 +5793,7 @@
         <v>142</v>
       </c>
       <c r="P38" s="8">
-        <f>100000/K38</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
       <c r="Q38" s="9" t="s">
@@ -5791,7 +5850,7 @@
         <v>142</v>
       </c>
       <c r="P39" s="8">
-        <f>100000/K39</f>
+        <f t="shared" si="1"/>
         <v>100000</v>
       </c>
       <c r="Q39" s="9" t="s">
@@ -6696,7 +6755,7 @@
         <v>258</v>
       </c>
       <c r="P55" s="8">
-        <f t="shared" ref="P55:P60" si="1">100000000/K55</f>
+        <f t="shared" ref="P55:P60" si="2">100000000/K55</f>
         <v>142.85714285714286</v>
       </c>
       <c r="Q55" s="9" t="s">
@@ -6759,7 +6818,7 @@
         <v>258</v>
       </c>
       <c r="P56" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>172.41379310344828</v>
       </c>
       <c r="Q56" s="9" t="s">
@@ -6822,7 +6881,7 @@
         <v>258</v>
       </c>
       <c r="P57" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>367.64705882352939</v>
       </c>
       <c r="Q57" s="9" t="s">
@@ -6885,7 +6944,7 @@
         <v>258</v>
       </c>
       <c r="P58" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>367.64705882352939</v>
       </c>
       <c r="Q58" s="9" t="s">
@@ -6948,7 +7007,7 @@
         <v>258</v>
       </c>
       <c r="P59" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4000</v>
       </c>
       <c r="Q59" s="9" t="s">
@@ -7011,7 +7070,7 @@
         <v>258</v>
       </c>
       <c r="P60" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>500</v>
       </c>
       <c r="Q60" s="9" t="s">

</xml_diff>